<commit_message>
Added support of tracking motor duty cycle in software.
</commit_message>
<xml_diff>
--- a/pin_mappings.xlsx
+++ b/pin_mappings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Standard Account\Desktop\College\6th sem\System Integration\Project\Code versions\DroneProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFD04EED-FEB6-4CD6-8100-033E2F4A17AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{897E1495-089D-4FB0-A70B-1D161ED8F200}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="396" yWindow="504" windowWidth="13872" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="44">
   <si>
     <t>TM4C Peripherals</t>
   </si>
@@ -130,6 +130,33 @@
   </si>
   <si>
     <t>3904(Base) - &gt; PC7 (GPIO)</t>
+  </si>
+  <si>
+    <t>ESCs</t>
+  </si>
+  <si>
+    <t>Motor 1</t>
+  </si>
+  <si>
+    <t>Motor 2</t>
+  </si>
+  <si>
+    <t>Motor 3</t>
+  </si>
+  <si>
+    <t>Motor 4</t>
+  </si>
+  <si>
+    <t>PA6</t>
+  </si>
+  <si>
+    <t>PA7</t>
+  </si>
+  <si>
+    <t>PB6</t>
+  </si>
+  <si>
+    <t>PB7</t>
   </si>
 </sst>
 </file>
@@ -447,10 +474,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:F35"/>
+  <dimension ref="B1:F44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -458,7 +485,7 @@
     <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.77734375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:6" x14ac:dyDescent="0.3">
@@ -655,6 +682,41 @@
         <v>15</v>
       </c>
     </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B41" t="s">
+        <v>35</v>
+      </c>
+      <c r="E41" t="s">
+        <v>36</v>
+      </c>
+      <c r="F41" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="E42" t="s">
+        <v>37</v>
+      </c>
+      <c r="F42" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="E43" t="s">
+        <v>38</v>
+      </c>
+      <c r="F43" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="E44" t="s">
+        <v>39</v>
+      </c>
+      <c r="F44" t="s">
+        <v>43</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Initial Altitude_adjust P block. Only PV and SP extracted. The main control algorithm is not yet implemented.
</commit_message>
<xml_diff>
--- a/pin_mappings.xlsx
+++ b/pin_mappings.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Standard Account\Desktop\College\6th sem\System Integration\Project\Code versions\DroneProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{897E1495-089D-4FB0-A70B-1D161ED8F200}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFEB1625-6532-47F4-B68C-D4C9C595F486}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="50">
   <si>
     <t>TM4C Peripherals</t>
   </si>
@@ -157,6 +157,24 @@
   </si>
   <si>
     <t>PB7</t>
+  </si>
+  <si>
+    <t>Orange RX</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> + </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - </t>
+  </si>
+  <si>
+    <t>5V</t>
+  </si>
+  <si>
+    <t>PD6</t>
+  </si>
+  <si>
+    <t>Signal (PPM)</t>
   </si>
 </sst>
 </file>
@@ -474,17 +492,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:F44"/>
+  <dimension ref="B1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="F45" sqref="F45"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.88671875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -717,6 +735,33 @@
         <v>43</v>
       </c>
     </row>
+    <row r="47" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B47" t="s">
+        <v>44</v>
+      </c>
+      <c r="E47" t="s">
+        <v>49</v>
+      </c>
+      <c r="F47" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="E48" t="s">
+        <v>45</v>
+      </c>
+      <c r="F48" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E49" t="s">
+        <v>46</v>
+      </c>
+      <c r="F49" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>